<commit_message>
Dernière version des slides, docs et codes
</commit_message>
<xml_diff>
--- a/output/notes_RESF_generees/tables/Tableau_RESF_2020_1.xlsx
+++ b/output/notes_RESF_generees/tables/Tableau_RESF_2020_1.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:D18"/>
+  <dimension ref="A1:G4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -441,17 +441,32 @@
       </c>
       <c r="B1" s="1" t="inlineStr">
         <is>
-          <t>Solde Public (en % du PIB)</t>
+          <t>PIB (%)</t>
         </is>
       </c>
       <c r="C1" s="1" t="inlineStr">
         <is>
-          <t>Dépense Publique hors CI (en % du PIB)</t>
+          <t>IPC (%)</t>
         </is>
       </c>
       <c r="D1" s="1" t="inlineStr">
         <is>
-          <t>Évolution en Volume (en %)</t>
+          <t>Solde Public (%)</t>
+        </is>
+      </c>
+      <c r="E1" s="1" t="inlineStr">
+        <is>
+          <t>Dette Publique Totale (%)</t>
+        </is>
+      </c>
+      <c r="F1" s="1" t="inlineStr">
+        <is>
+          <t>Dépenses Publiques (%)</t>
+        </is>
+      </c>
+      <c r="G1" s="1" t="inlineStr">
+        <is>
+          <t>Prélèvements Obligatoires (%)</t>
         </is>
       </c>
     </row>
@@ -463,335 +478,108 @@
       </c>
       <c r="B2" t="inlineStr">
         <is>
+          <t>--------</t>
+        </is>
+      </c>
+      <c r="C2" t="inlineStr">
+        <is>
+          <t>---------</t>
+        </is>
+      </c>
+      <c r="D2" t="inlineStr">
+        <is>
+          <t>------------------</t>
+        </is>
+      </c>
+      <c r="E2" t="inlineStr">
+        <is>
           <t>---------------------------</t>
         </is>
       </c>
-      <c r="C2" t="inlineStr">
-        <is>
-          <t>---------------------------------------</t>
-        </is>
-      </c>
-      <c r="D2" t="inlineStr">
-        <is>
-          <t>----------------------------</t>
+      <c r="F2" t="inlineStr">
+        <is>
+          <t>------------------------</t>
+        </is>
+      </c>
+      <c r="G2" t="inlineStr">
+        <is>
+          <t>------------------------------</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>2017</t>
+          <t>2019</t>
         </is>
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>-2,8</t>
+          <t>1,4</t>
         </is>
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>55,0</t>
+          <t>1,3</t>
         </is>
       </c>
       <c r="D3" t="inlineStr">
         <is>
-          <t>1,4</t>
+          <t>-3,1</t>
+        </is>
+      </c>
+      <c r="E3" t="inlineStr">
+        <is>
+          <t>98,8</t>
+        </is>
+      </c>
+      <c r="F3" t="inlineStr">
+        <is>
+          <t>53,8</t>
+        </is>
+      </c>
+      <c r="G3" t="inlineStr">
+        <is>
+          <t>44,0</t>
         </is>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>2018</t>
+          <t>2020</t>
         </is>
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>-2,5</t>
+          <t>1,3</t>
         </is>
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>54,4</t>
+          <t>1,3</t>
         </is>
       </c>
       <c r="D4" t="inlineStr">
         <is>
-          <t>-0,3</t>
-        </is>
-      </c>
-    </row>
-    <row r="5">
-      <c r="A5" t="inlineStr">
-        <is>
-          <t>2019</t>
-        </is>
-      </c>
-      <c r="B5" t="inlineStr">
-        <is>
-          <t>-3,1</t>
-        </is>
-      </c>
-      <c r="C5" t="inlineStr">
-        <is>
-          <t>53,8</t>
-        </is>
-      </c>
-      <c r="D5" t="inlineStr">
-        <is>
-          <t>0,7</t>
-        </is>
-      </c>
-    </row>
-    <row r="6">
-      <c r="A6" t="inlineStr">
-        <is>
-          <t>2020</t>
-        </is>
-      </c>
-      <c r="B6" t="inlineStr">
-        <is>
           <t>-2,2</t>
         </is>
       </c>
-      <c r="C6" t="inlineStr">
+      <c r="E4" t="inlineStr">
+        <is>
+          <t>98,7</t>
+        </is>
+      </c>
+      <c r="F4" t="inlineStr">
         <is>
           <t>53,4</t>
         </is>
       </c>
-      <c r="D6" t="inlineStr">
-        <is>
-          <t>0,7</t>
-        </is>
-      </c>
-    </row>
-    <row r="7">
-      <c r="A7" t="inlineStr">
-        <is>
-          <t>2021</t>
-        </is>
-      </c>
-      <c r="B7" t="inlineStr">
-        <is>
-          <t>-1,8</t>
-        </is>
-      </c>
-      <c r="C7" t="inlineStr">
-        <is>
-          <t>52,9</t>
-        </is>
-      </c>
-      <c r="D7" t="inlineStr">
-        <is>
-          <t>0,5</t>
-        </is>
-      </c>
-    </row>
-    <row r="8">
-      <c r="A8" t="inlineStr">
-        <is>
-          <t>2022</t>
-        </is>
-      </c>
-      <c r="B8" t="inlineStr">
-        <is>
-          <t>-1,5</t>
-        </is>
-      </c>
-      <c r="C8" t="inlineStr">
-        <is>
-          <t>52,3</t>
-        </is>
-      </c>
-      <c r="D8" t="inlineStr">
-        <is>
-          <t>0,2</t>
-        </is>
-      </c>
-    </row>
-    <row r="9">
-      <c r="A9" t="inlineStr">
-        <is>
-          <t>2023</t>
-        </is>
-      </c>
-      <c r="B9" t="inlineStr">
-        <is>
-          <t>-1,1</t>
-        </is>
-      </c>
-      <c r="C9" t="inlineStr">
-        <is>
-          <t>51,9</t>
-        </is>
-      </c>
-      <c r="D9" t="inlineStr">
-        <is>
-          <t>0,4</t>
-        </is>
-      </c>
-    </row>
-    <row r="10">
-      <c r="A10" t="inlineStr">
-        <is>
-          <t>Année</t>
-        </is>
-      </c>
-      <c r="B10" t="inlineStr">
-        <is>
-          <t>Dette Publique Totale (en % du PIB)</t>
-        </is>
-      </c>
-      <c r="C10" t="inlineStr">
-        <is>
-          <t>Dette Publique hors Soutien à la Zone Euro (en % du PIB)</t>
-        </is>
-      </c>
-      <c r="D10" t="inlineStr"/>
-    </row>
-    <row r="11">
-      <c r="A11" t="inlineStr">
-        <is>
-          <t>-------</t>
-        </is>
-      </c>
-      <c r="B11" t="inlineStr">
-        <is>
-          <t>--------------------------------------</t>
-        </is>
-      </c>
-      <c r="C11" t="inlineStr">
-        <is>
-          <t>---------------------------------------------------------</t>
-        </is>
-      </c>
-      <c r="D11" t="inlineStr"/>
-    </row>
-    <row r="12">
-      <c r="A12" t="inlineStr">
-        <is>
-          <t>2018</t>
-        </is>
-      </c>
-      <c r="B12" t="inlineStr">
-        <is>
-          <t>98,4</t>
-        </is>
-      </c>
-      <c r="C12" t="inlineStr">
-        <is>
-          <t>95,6</t>
-        </is>
-      </c>
-      <c r="D12" t="inlineStr"/>
-    </row>
-    <row r="13">
-      <c r="A13" t="inlineStr">
-        <is>
-          <t>2019</t>
-        </is>
-      </c>
-      <c r="B13" t="inlineStr">
-        <is>
-          <t>98,8</t>
-        </is>
-      </c>
-      <c r="C13" t="inlineStr">
-        <is>
-          <t>96,1</t>
-        </is>
-      </c>
-      <c r="D13" t="inlineStr"/>
-    </row>
-    <row r="14">
-      <c r="A14" t="inlineStr">
-        <is>
-          <t>2020</t>
-        </is>
-      </c>
-      <c r="B14" t="inlineStr">
-        <is>
-          <t>98,7</t>
-        </is>
-      </c>
-      <c r="C14" t="inlineStr">
-        <is>
-          <t>96,1</t>
-        </is>
-      </c>
-      <c r="D14" t="inlineStr"/>
-    </row>
-    <row r="15">
-      <c r="A15" t="inlineStr">
-        <is>
-          <t>Année</t>
-        </is>
-      </c>
-      <c r="B15" t="inlineStr">
-        <is>
-          <t>Croissance du PIB (en %)</t>
-        </is>
-      </c>
-      <c r="C15" t="inlineStr">
-        <is>
-          <t>Inflation (IPC, en %)</t>
-        </is>
-      </c>
-      <c r="D15" t="inlineStr"/>
-    </row>
-    <row r="16">
-      <c r="A16" t="inlineStr">
-        <is>
-          <t>-------</t>
-        </is>
-      </c>
-      <c r="B16" t="inlineStr">
-        <is>
-          <t>---------------------------</t>
-        </is>
-      </c>
-      <c r="C16" t="inlineStr">
-        <is>
-          <t>-----------------------</t>
-        </is>
-      </c>
-      <c r="D16" t="inlineStr"/>
-    </row>
-    <row r="17">
-      <c r="A17" t="inlineStr">
-        <is>
-          <t>2019</t>
-        </is>
-      </c>
-      <c r="B17" t="inlineStr">
-        <is>
-          <t>1,4</t>
-        </is>
-      </c>
-      <c r="C17" t="inlineStr">
-        <is>
-          <t>1,3</t>
-        </is>
-      </c>
-      <c r="D17" t="inlineStr"/>
-    </row>
-    <row r="18">
-      <c r="A18" t="inlineStr">
-        <is>
-          <t>2020</t>
-        </is>
-      </c>
-      <c r="B18" t="inlineStr">
-        <is>
-          <t>1,3</t>
-        </is>
-      </c>
-      <c r="C18" t="inlineStr">
-        <is>
-          <t>1,3</t>
-        </is>
-      </c>
-      <c r="D18" t="inlineStr"/>
+      <c r="G4" t="inlineStr">
+        <is>
+          <t>44,3</t>
+        </is>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>